<commit_message>
updated Jupyter NB, README file and nybrews_corrections.xlsx
</commit_message>
<xml_diff>
--- a/nybrews corrections.xlsx
+++ b/nybrews corrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\GitHub\ETL-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D528A713-C838-49F9-8E28-C71EEC7DA2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D09A685-FE42-4CDB-8A96-29ED5480952C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="225" windowWidth="21600" windowHeight="11385" xr2:uid="{B04FB94C-9D3A-403C-B830-0F759644F9CC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B04FB94C-9D3A-403C-B830-0F759644F9CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="23">
   <si>
     <t>Nacho Mama's Brewery</t>
   </si>
@@ -96,17 +96,38 @@
     <t xml:space="preserve"> Chelsea Piers</t>
   </si>
   <si>
-    <t>The Radius of the Earth is 3960 miles and 1 mile = 5280 feet.</t>
+    <t>Corrected Data</t>
+  </si>
+  <si>
+    <t>Data to be scrubbed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,12 +165,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1163C9-3049-4D8E-8C81-5986536624A4}">
-  <dimension ref="A5:G22"/>
+  <dimension ref="A5:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,9 +504,10 @@
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -496,7 +524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>34</v>
       </c>
@@ -510,8 +538,11 @@
         <v>14</v>
       </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>44</v>
       </c>
@@ -527,8 +558,9 @@
       <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>81</v>
       </c>
@@ -544,8 +576,9 @@
       <c r="E8" s="3">
         <v>11746</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>82</v>
       </c>
@@ -561,8 +594,9 @@
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>34</v>
       </c>
@@ -578,8 +612,11 @@
       <c r="E11" s="4">
         <v>10013</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>44</v>
       </c>
@@ -595,8 +632,9 @@
       <c r="E12" s="4">
         <v>13206</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>81</v>
       </c>
@@ -612,8 +650,9 @@
       <c r="E13" s="4">
         <v>11746</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>82</v>
       </c>
@@ -629,37 +668,14 @@
       <c r="E14" s="4">
         <v>10011</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>3960</v>
-      </c>
-      <c r="D20">
-        <v>5280</v>
-      </c>
-      <c r="E20">
-        <f>D20*C20</f>
-        <v>20908800</v>
-      </c>
-      <c r="G20">
-        <f>E20/3</f>
-        <v>6969600</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <v>20908800</v>
-      </c>
-      <c r="G22">
-        <v>6969600</v>
-      </c>
+      <c r="F14" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F11:F14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>